<commit_message>
Add assembled pictures of all modules, adjust some BOMs to not use female headers.
</commit_message>
<xml_diff>
--- a/Modules/MiX/MiX_BOM.xlsx
+++ b/Modules/MiX/MiX_BOM.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\MiX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CD5299-DBFB-4EB5-8116-6D75E1E44ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiX_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>Qty</t>
   </si>
@@ -226,17 +245,206 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>P_VOL1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_VOL2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_VOL3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, C2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>* Place electrolytic capacitors sideways off the edge of the board.</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005002670881002.html</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/cm-100n-x7r_100/mlcc-tht-capacitors/sr-passives/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/jrg-47u_35/tht-electrolytic-capacitors/jb-capacitors/jrg1v470m02500630115000b/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/1n4001-dio/tht-universal-diodes/diotec-semiconductor/1n4001/</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003256812123.html</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/tl072ip/tht-operational-amplifiers/texas-instruments/</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/ttpots/</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/thonkiconn/</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Pushernut</t>
+  </si>
+  <si>
+    <t>Jack Nut</t>
+  </si>
+  <si>
+    <t>https://pushermanproductions.com/product/black-smooth-edge-jack-nuts-pack-of-25/</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>https://pushermanproductions.com/product/pushernuts-gold-smooth-edge-jack-nuts-pack-of-25/</t>
+  </si>
+  <si>
+    <t>Thonk Trimmer Topper</t>
+  </si>
+  <si>
+    <t>Trimmer Knob</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/tall-trimmer-toppers/</t>
+  </si>
+  <si>
+    <t>** Cut the legs of the header below P_VOL1 and P_VOL3 so they don't short.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>J_B1</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,</t>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -245,256 +453,31 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> J_B2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_VOL1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_VOL2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_VOL3</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>C1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, C2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>* Place electrolytic capacitors sideways off the edge of the board.</t>
-  </si>
-  <si>
-    <r>
-      <t>J_A1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>***</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, J_A2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>***</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005002670881002.html</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/cm-100n-x7r_100/mlcc-tht-capacitors/sr-passives/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/jrg-47u_35/tht-electrolytic-capacitors/jb-capacitors/jrg1v470m02500630115000b/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/1n4001-dio/tht-universal-diodes/diotec-semiconductor/1n4001/</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005003256812123.html</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/tl072ip/tht-operational-amplifiers/texas-instruments/</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/ttpots/</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/thonkiconn/</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005001557138121.html</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Pushernut</t>
-  </si>
-  <si>
-    <t>Jack Nut</t>
-  </si>
-  <si>
-    <t>https://pushermanproductions.com/product/black-smooth-edge-jack-nuts-pack-of-25/</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>https://pushermanproductions.com/product/pushernuts-gold-smooth-edge-jack-nuts-pack-of-25/</t>
-  </si>
-  <si>
-    <t>Thonk Trimmer Topper</t>
-  </si>
-  <si>
-    <t>Trimmer Knob</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/tall-trimmer-toppers/</t>
-  </si>
-  <si>
-    <t>** Cut the legs of the header below P_VOL1 and P_VOL3 so they don't short.</t>
-  </si>
-  <si>
-    <r>
-      <t>Female Header 2.54mm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>***</t>
-    </r>
-  </si>
-  <si>
-    <t>*** You may omit the female headers and solder the angled headers directly to front PCB for stability. If using the female headers, remove the plastic base on headers J_A1 and J_A2 to make the board more flush with the 2hp and trim the extra leg length after soldering.</t>
+  </si>
+  <si>
+    <t>*** Solder the plastic side of the angled header on the J_B side, and the metal on J_A side. Cut off the excess length.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -693,11 +676,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1088,7 +1071,7 @@
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="43"/>
+    <cellStyle name="Hyperlink 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1105,14 +1088,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1150,7 +1136,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1222,7 +1208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1395,11 +1381,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,7 +1434,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1468,7 +1454,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,7 +1474,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1502,13 +1488,13 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,7 +1514,7 @@
         <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1548,7 +1534,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1568,7 +1554,7 @@
         <v>28</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1582,13 +1568,13 @@
         <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,7 +1594,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1622,7 +1608,7 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
@@ -1645,113 +1631,92 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>57</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="5" t="s">
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2:F3" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F17" r:id="rId10"/>
-    <hyperlink ref="F15" r:id="rId11"/>
-    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F2:F3" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>